<commit_message>
Added visualizations and recommendation results
</commit_message>
<xml_diff>
--- a/results_new/hdbscan.xlsx
+++ b/results_new/hdbscan.xlsx
@@ -455,7 +455,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3">
@@ -468,7 +468,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4">
@@ -481,7 +481,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5">
@@ -494,7 +494,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6">
@@ -507,7 +507,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="7">
@@ -520,7 +520,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -533,7 +533,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9">
@@ -546,7 +546,7 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="10">
@@ -559,7 +559,7 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11">
@@ -572,7 +572,7 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12">
@@ -585,7 +585,7 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="13">
@@ -598,7 +598,7 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="14">
@@ -611,7 +611,7 @@
         </is>
       </c>
       <c r="C14" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15">
@@ -624,7 +624,7 @@
         </is>
       </c>
       <c r="C15" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16">
@@ -637,7 +637,7 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -650,7 +650,7 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18">
@@ -663,7 +663,7 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="19">
@@ -676,7 +676,7 @@
         </is>
       </c>
       <c r="C19" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20">
@@ -689,7 +689,7 @@
         </is>
       </c>
       <c r="C20" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21">
@@ -702,7 +702,7 @@
         </is>
       </c>
       <c r="C21" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="22">
@@ -715,7 +715,7 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23">
@@ -728,7 +728,7 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24">
@@ -741,7 +741,7 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25">
@@ -754,7 +754,7 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26">
@@ -767,7 +767,7 @@
         </is>
       </c>
       <c r="C26" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="27">
@@ -780,7 +780,7 @@
         </is>
       </c>
       <c r="C27" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28">
@@ -793,7 +793,7 @@
         </is>
       </c>
       <c r="C28" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29">
@@ -806,7 +806,7 @@
         </is>
       </c>
       <c r="C29" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="30">
@@ -819,7 +819,7 @@
         </is>
       </c>
       <c r="C30" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31">
@@ -832,7 +832,7 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="32">
@@ -845,7 +845,7 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="33">
@@ -858,7 +858,7 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="34">
@@ -871,7 +871,7 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="35">
@@ -884,7 +884,7 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36">
@@ -897,7 +897,7 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="37">
@@ -910,7 +910,7 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38">
@@ -923,7 +923,7 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="39">
@@ -936,7 +936,7 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="40">
@@ -949,7 +949,7 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="41">
@@ -962,7 +962,7 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="42">
@@ -975,7 +975,7 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43">
@@ -988,7 +988,7 @@
         </is>
       </c>
       <c r="C43" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="44">
@@ -1001,7 +1001,7 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="45">
@@ -1014,7 +1014,7 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46">
@@ -1027,7 +1027,7 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="47">
@@ -1040,7 +1040,7 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="48">
@@ -1053,7 +1053,7 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="49">
@@ -1066,7 +1066,7 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="50">
@@ -1079,7 +1079,7 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="51">
@@ -1092,7 +1092,7 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="52">
@@ -1105,7 +1105,7 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53">
@@ -1118,7 +1118,7 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="54">
@@ -1131,7 +1131,7 @@
         </is>
       </c>
       <c r="C54" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="55">
@@ -1144,7 +1144,7 @@
         </is>
       </c>
       <c r="C55" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56">
@@ -1157,7 +1157,7 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="57">
@@ -1170,7 +1170,7 @@
         </is>
       </c>
       <c r="C57" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="58">
@@ -1183,7 +1183,7 @@
         </is>
       </c>
       <c r="C58" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="59">
@@ -1196,7 +1196,7 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="60">
@@ -1209,7 +1209,7 @@
         </is>
       </c>
       <c r="C60" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="61">
@@ -1222,7 +1222,7 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="62">
@@ -1235,7 +1235,7 @@
         </is>
       </c>
       <c r="C62" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63">
@@ -1248,7 +1248,7 @@
         </is>
       </c>
       <c r="C63" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="64">
@@ -1261,7 +1261,7 @@
         </is>
       </c>
       <c r="C64" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="65">
@@ -1274,7 +1274,7 @@
         </is>
       </c>
       <c r="C65" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="66">
@@ -1287,7 +1287,7 @@
         </is>
       </c>
       <c r="C66" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="67">
@@ -1300,7 +1300,7 @@
         </is>
       </c>
       <c r="C67" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="68">
@@ -1313,7 +1313,7 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="69">
@@ -1326,7 +1326,7 @@
         </is>
       </c>
       <c r="C69" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="70">
@@ -1339,7 +1339,7 @@
         </is>
       </c>
       <c r="C70" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="71">
@@ -1352,7 +1352,7 @@
         </is>
       </c>
       <c r="C71" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="72">
@@ -1365,7 +1365,7 @@
         </is>
       </c>
       <c r="C72" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="73">
@@ -1378,7 +1378,7 @@
         </is>
       </c>
       <c r="C73" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="74">
@@ -1391,7 +1391,7 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="75">
@@ -1404,7 +1404,7 @@
         </is>
       </c>
       <c r="C75" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="76">
@@ -1417,7 +1417,7 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="77">
@@ -1430,7 +1430,7 @@
         </is>
       </c>
       <c r="C77" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="78">
@@ -1443,7 +1443,7 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="79">
@@ -1456,7 +1456,7 @@
         </is>
       </c>
       <c r="C79" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="80">
@@ -1469,7 +1469,7 @@
         </is>
       </c>
       <c r="C80" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="81">
@@ -1482,7 +1482,7 @@
         </is>
       </c>
       <c r="C81" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="82">
@@ -1495,7 +1495,7 @@
         </is>
       </c>
       <c r="C82" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="83">
@@ -1508,7 +1508,7 @@
         </is>
       </c>
       <c r="C83" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="84">
@@ -1521,7 +1521,7 @@
         </is>
       </c>
       <c r="C84" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="85">
@@ -1534,7 +1534,7 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="86">
@@ -1547,7 +1547,7 @@
         </is>
       </c>
       <c r="C86" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="87">
@@ -1560,7 +1560,7 @@
         </is>
       </c>
       <c r="C87" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="88">
@@ -1573,7 +1573,7 @@
         </is>
       </c>
       <c r="C88" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="89">
@@ -1586,7 +1586,7 @@
         </is>
       </c>
       <c r="C89" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="90">
@@ -1599,7 +1599,7 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="91">
@@ -1612,7 +1612,7 @@
         </is>
       </c>
       <c r="C91" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="92">
@@ -1625,7 +1625,7 @@
         </is>
       </c>
       <c r="C92" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="93">
@@ -1638,7 +1638,7 @@
         </is>
       </c>
       <c r="C93" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="94">
@@ -1651,7 +1651,7 @@
         </is>
       </c>
       <c r="C94" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="95">
@@ -1664,7 +1664,7 @@
         </is>
       </c>
       <c r="C95" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="96">
@@ -1677,7 +1677,7 @@
         </is>
       </c>
       <c r="C96" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="97">
@@ -1690,7 +1690,7 @@
         </is>
       </c>
       <c r="C97" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="98">
@@ -1703,7 +1703,7 @@
         </is>
       </c>
       <c r="C98" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="99">
@@ -1716,7 +1716,7 @@
         </is>
       </c>
       <c r="C99" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="100">
@@ -1729,7 +1729,7 @@
         </is>
       </c>
       <c r="C100" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="101">
@@ -1742,7 +1742,7 @@
         </is>
       </c>
       <c r="C101" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="102">
@@ -1755,7 +1755,7 @@
         </is>
       </c>
       <c r="C102" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="103">
@@ -1768,7 +1768,7 @@
         </is>
       </c>
       <c r="C103" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="104">
@@ -1781,7 +1781,7 @@
         </is>
       </c>
       <c r="C104" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="105">
@@ -1794,7 +1794,7 @@
         </is>
       </c>
       <c r="C105" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="106">
@@ -1807,7 +1807,7 @@
         </is>
       </c>
       <c r="C106" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="107">
@@ -1820,7 +1820,7 @@
         </is>
       </c>
       <c r="C107" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="108">
@@ -1833,7 +1833,7 @@
         </is>
       </c>
       <c r="C108" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="109">
@@ -1846,7 +1846,7 @@
         </is>
       </c>
       <c r="C109" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="110">
@@ -1859,7 +1859,7 @@
         </is>
       </c>
       <c r="C110" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="111">
@@ -1872,7 +1872,7 @@
         </is>
       </c>
       <c r="C111" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="112">
@@ -1885,7 +1885,7 @@
         </is>
       </c>
       <c r="C112" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="113">
@@ -1898,7 +1898,7 @@
         </is>
       </c>
       <c r="C113" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="114">
@@ -1911,7 +1911,7 @@
         </is>
       </c>
       <c r="C114" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="115">
@@ -1924,7 +1924,7 @@
         </is>
       </c>
       <c r="C115" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="116">
@@ -1937,7 +1937,7 @@
         </is>
       </c>
       <c r="C116" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="117">
@@ -1950,7 +1950,7 @@
         </is>
       </c>
       <c r="C117" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="118">
@@ -1963,7 +1963,7 @@
         </is>
       </c>
       <c r="C118" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="119">
@@ -1976,7 +1976,7 @@
         </is>
       </c>
       <c r="C119" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="120">
@@ -2002,7 +2002,7 @@
         </is>
       </c>
       <c r="C121" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="122">
@@ -2015,7 +2015,7 @@
         </is>
       </c>
       <c r="C122" t="n">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="123">
@@ -2028,7 +2028,7 @@
         </is>
       </c>
       <c r="C123" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="124">
@@ -2041,7 +2041,7 @@
         </is>
       </c>
       <c r="C124" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="125">
@@ -2054,7 +2054,7 @@
         </is>
       </c>
       <c r="C125" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="126">
@@ -2067,7 +2067,7 @@
         </is>
       </c>
       <c r="C126" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="127">
@@ -2080,7 +2080,7 @@
         </is>
       </c>
       <c r="C127" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="128">
@@ -2093,7 +2093,7 @@
         </is>
       </c>
       <c r="C128" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="129">
@@ -2106,7 +2106,7 @@
         </is>
       </c>
       <c r="C129" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="130">
@@ -2119,7 +2119,7 @@
         </is>
       </c>
       <c r="C130" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="131">
@@ -2132,7 +2132,7 @@
         </is>
       </c>
       <c r="C131" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="132">
@@ -2145,7 +2145,7 @@
         </is>
       </c>
       <c r="C132" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="133">
@@ -2158,7 +2158,7 @@
         </is>
       </c>
       <c r="C133" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="134">
@@ -2171,7 +2171,7 @@
         </is>
       </c>
       <c r="C134" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="135">
@@ -2184,7 +2184,7 @@
         </is>
       </c>
       <c r="C135" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="136">
@@ -2197,7 +2197,7 @@
         </is>
       </c>
       <c r="C136" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="137">
@@ -2210,7 +2210,7 @@
         </is>
       </c>
       <c r="C137" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="138">
@@ -2223,7 +2223,7 @@
         </is>
       </c>
       <c r="C138" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="139">
@@ -2236,7 +2236,7 @@
         </is>
       </c>
       <c r="C139" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="140">
@@ -2249,7 +2249,7 @@
         </is>
       </c>
       <c r="C140" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="141">
@@ -2262,7 +2262,7 @@
         </is>
       </c>
       <c r="C141" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="142">
@@ -2275,7 +2275,7 @@
         </is>
       </c>
       <c r="C142" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="143">
@@ -2288,7 +2288,7 @@
         </is>
       </c>
       <c r="C143" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="144">
@@ -2301,7 +2301,7 @@
         </is>
       </c>
       <c r="C144" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="145">
@@ -2314,7 +2314,7 @@
         </is>
       </c>
       <c r="C145" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="146">
@@ -2327,7 +2327,7 @@
         </is>
       </c>
       <c r="C146" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="147">
@@ -2340,7 +2340,7 @@
         </is>
       </c>
       <c r="C147" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="148">
@@ -2353,7 +2353,7 @@
         </is>
       </c>
       <c r="C148" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="149">
@@ -2366,7 +2366,7 @@
         </is>
       </c>
       <c r="C149" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="150">
@@ -2379,7 +2379,7 @@
         </is>
       </c>
       <c r="C150" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="151">
@@ -2392,7 +2392,7 @@
         </is>
       </c>
       <c r="C151" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="152">
@@ -2405,7 +2405,7 @@
         </is>
       </c>
       <c r="C152" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="153">
@@ -2418,7 +2418,7 @@
         </is>
       </c>
       <c r="C153" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="154">
@@ -2431,7 +2431,7 @@
         </is>
       </c>
       <c r="C154" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="155">
@@ -2444,7 +2444,7 @@
         </is>
       </c>
       <c r="C155" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="156">
@@ -2457,7 +2457,7 @@
         </is>
       </c>
       <c r="C156" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="157">
@@ -2470,7 +2470,7 @@
         </is>
       </c>
       <c r="C157" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="158">
@@ -2483,7 +2483,7 @@
         </is>
       </c>
       <c r="C158" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="159">
@@ -2496,7 +2496,7 @@
         </is>
       </c>
       <c r="C159" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="160">
@@ -2509,7 +2509,7 @@
         </is>
       </c>
       <c r="C160" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="161">
@@ -2522,7 +2522,7 @@
         </is>
       </c>
       <c r="C161" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="162">
@@ -2535,7 +2535,7 @@
         </is>
       </c>
       <c r="C162" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="163">
@@ -2548,7 +2548,7 @@
         </is>
       </c>
       <c r="C163" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="164">
@@ -2561,7 +2561,7 @@
         </is>
       </c>
       <c r="C164" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="165">
@@ -2574,7 +2574,7 @@
         </is>
       </c>
       <c r="C165" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="166">
@@ -2587,7 +2587,7 @@
         </is>
       </c>
       <c r="C166" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="167">
@@ -2600,7 +2600,7 @@
         </is>
       </c>
       <c r="C167" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="168">
@@ -2613,7 +2613,7 @@
         </is>
       </c>
       <c r="C168" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="169">
@@ -2626,7 +2626,7 @@
         </is>
       </c>
       <c r="C169" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="170">
@@ -2639,7 +2639,7 @@
         </is>
       </c>
       <c r="C170" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="171">
@@ -2652,7 +2652,7 @@
         </is>
       </c>
       <c r="C171" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="172">
@@ -2665,7 +2665,7 @@
         </is>
       </c>
       <c r="C172" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="173">
@@ -2678,7 +2678,7 @@
         </is>
       </c>
       <c r="C173" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="174">
@@ -2691,7 +2691,7 @@
         </is>
       </c>
       <c r="C174" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
     <row r="175">
@@ -2704,7 +2704,7 @@
         </is>
       </c>
       <c r="C175" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="176">
@@ -2717,7 +2717,7 @@
         </is>
       </c>
       <c r="C176" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="177">
@@ -2730,7 +2730,7 @@
         </is>
       </c>
       <c r="C177" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="178">
@@ -2743,7 +2743,7 @@
         </is>
       </c>
       <c r="C178" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="179">
@@ -2756,7 +2756,7 @@
         </is>
       </c>
       <c r="C179" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="180">
@@ -2769,7 +2769,7 @@
         </is>
       </c>
       <c r="C180" t="n">
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>